<commit_message>
Problem 170LBabbar sheet done
</commit_message>
<xml_diff>
--- a/Problems/Final450/FINAL450.xlsx
+++ b/Problems/Final450/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\vdcodes\Programming\DSA\Problems\Final450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1AF188-D68F-4104-BC0E-4A4775751AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4297897-40E5-41B6-8E20-5DCCECFB6EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A174" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A162" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4328,7 +4328,7 @@
       <c r="B185" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C185" s="12" t="s">
+      <c r="C185" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D185">

</xml_diff>